<commit_message>
ok had to fix typo
</commit_message>
<xml_diff>
--- a/graphicsExcels/Weekly Sale.xlsx
+++ b/graphicsExcels/Weekly Sale.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annax/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annax/Desktop/soupysoup/graphicsExcels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A5FE4C-4BEC-3642-B7D1-C14CD6E2B1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DF6595-E892-5E4A-9EB2-3718137C58C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="2800" windowWidth="15920" windowHeight="13160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,13 +572,13 @@
     <t>ichiban tofu</t>
   </si>
   <si>
-    <t>cbinese name</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>chinese name</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1333,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1346,16 +1346,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>